<commit_message>
I ran the outside-only wearable vs weather data on both the MLP and LR
</commit_message>
<xml_diff>
--- a/Data_Folder/Wearable_Sensor_Data.xlsx
+++ b/Data_Folder/Wearable_Sensor_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="8120" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="2580" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1778,8 +1778,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1818,7 +1820,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1829,6 +1831,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1839,6 +1842,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2174,7 +2178,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2226,10 +2230,7 @@
       <c r="A2" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="B2" s="1" t="str">
-        <f>TEXT(J2,"m/dd/yy")&amp;" "&amp;TEXT(K2,"hh:mm:ss")</f>
-        <v>3/04/19 20:37:02</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="11" t="s">
         <v>565</v>
       </c>

</xml_diff>